<commit_message>
Excel based driver code completed - GCMS code added to point of login
</commit_message>
<xml_diff>
--- a/Test_Data/TestData.xlsx
+++ b/Test_Data/TestData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCase" sheetId="1" r:id="rId1"/>
-    <sheet name="Env" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TestSchedule" r:id="rId1" sheetId="1"/>
+    <sheet name="TestCase" r:id="rId2" sheetId="4"/>
+    <sheet name="Env" r:id="rId3" sheetId="2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>URL</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Screenshot</t>
   </si>
   <si>
-    <t>C:/IdeaProjects/TestAuto/Results/</t>
-  </si>
-  <si>
     <t>Component_Name</t>
   </si>
   <si>
@@ -64,13 +61,53 @@
   </si>
   <si>
     <t>TestEnv</t>
+  </si>
+  <si>
+    <t>UAT1</t>
+  </si>
+  <si>
+    <t>Interchange_ID</t>
+  </si>
+  <si>
+    <t>TakeScreenShots</t>
+  </si>
+  <si>
+    <t>OPF12345678</t>
+  </si>
+  <si>
+    <t>Logout_BVA</t>
+  </si>
+  <si>
+    <t>H:\My Documents\Test Bench\IdeaProjects\TestAuto\Results\</t>
+  </si>
+  <si>
+    <t>GCMS</t>
+  </si>
+  <si>
+    <t>https://training-www2.ffrontier.com/gcms/FFrontier</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>Login_GCMS</t>
+  </si>
+  <si>
+    <t>UnitCode</t>
+  </si>
+  <si>
+    <t>MZ1</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,17 +142,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -124,10 +166,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -194,6 +236,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -228,6 +271,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -283,7 +327,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -292,13 +336,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -308,7 +352,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -317,7 +361,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -326,7 +370,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -336,12 +380,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -372,7 +416,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -391,7 +435,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -403,116 +447,206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row customFormat="1" r="1" s="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row customFormat="1" r="2" s="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="49.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="56.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to logging and screenshots, components added
</commit_message>
<xml_diff>
--- a/Test_Data/TestData.xlsx
+++ b/Test_Data/TestData.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSchedule" r:id="rId1" sheetId="1"/>
-    <sheet name="TestCase" r:id="rId2" sheetId="4"/>
-    <sheet name="Env" r:id="rId3" sheetId="2"/>
+    <sheet name="TestSchedule" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCase" sheetId="4" r:id="rId2"/>
+    <sheet name="Env" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="97">
   <si>
     <t>URL</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Password01</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>Screenshot</t>
   </si>
   <si>
@@ -66,48 +63,257 @@
     <t>UAT1</t>
   </si>
   <si>
-    <t>Interchange_ID</t>
-  </si>
-  <si>
-    <t>TakeScreenShots</t>
-  </si>
-  <si>
-    <t>OPF12345678</t>
-  </si>
-  <si>
     <t>Logout_BVA</t>
   </si>
   <si>
     <t>H:\My Documents\Test Bench\IdeaProjects\TestAuto\Results\</t>
   </si>
   <si>
-    <t>GCMS</t>
-  </si>
-  <si>
     <t>https://training-www2.ffrontier.com/gcms/FFrontier</t>
   </si>
   <si>
-    <t>TC002</t>
-  </si>
-  <si>
-    <t>Login_GCMS</t>
-  </si>
-  <si>
     <t>UnitCode</t>
   </si>
   <si>
-    <t>MZ1</t>
-  </si>
-  <si>
-    <t>Pass</t>
+    <t>GCMS_London</t>
+  </si>
+  <si>
+    <t>bartmi1</t>
+  </si>
+  <si>
+    <t>GCMS_Auto1</t>
+  </si>
+  <si>
+    <t>GCMS_Paris</t>
+  </si>
+  <si>
+    <t>GCMS_Amsterdam</t>
+  </si>
+  <si>
+    <t>03006017</t>
+  </si>
+  <si>
+    <t>08001061</t>
+  </si>
+  <si>
+    <t>https://v-esweb01t:9443/BankVisibility/</t>
+  </si>
+  <si>
+    <t>Choose_From_Menu</t>
+  </si>
+  <si>
+    <t>Manual Entry=&gt;SEPA=&gt;Manual Entry CCTI</t>
+  </si>
+  <si>
+    <t>Search_And_Load_Template</t>
+  </si>
+  <si>
+    <t>Execution_Date:Today</t>
+  </si>
+  <si>
+    <t>Enter_Credit_Party</t>
+  </si>
+  <si>
+    <t>Transaction_Information</t>
+  </si>
+  <si>
+    <t>End_To_End_Identification:xx999xx</t>
+  </si>
+  <si>
+    <t>Instructed_Amount_Currency:EUR</t>
+  </si>
+  <si>
+    <t>Enter_Remittance_Information</t>
+  </si>
+  <si>
+    <t>Currency:EUR - Euro</t>
+  </si>
+  <si>
+    <t>Validate_And_Enrich_Debit_Party</t>
+  </si>
+  <si>
+    <t>Instruction_Type:pain.001.001.03</t>
+  </si>
+  <si>
+    <t>Enter_Credit_Party_Agent</t>
+  </si>
+  <si>
+    <t>Branch:Mizuho London</t>
+  </si>
+  <si>
+    <t>Batch_Booking:No</t>
+  </si>
+  <si>
+    <t>Customer_Id:539459</t>
+  </si>
+  <si>
+    <t>Choose_Customer_IBAN</t>
+  </si>
+  <si>
+    <t>IBAN_Account_Number:GB60MHCB40506910804139</t>
+  </si>
+  <si>
+    <t>Name:AIP LONDON LIMITED</t>
+  </si>
+  <si>
+    <t>Address_Line_1:P &amp; CO  CHARTERED ACCOUNTANTS, LOND</t>
+  </si>
+  <si>
+    <t>Address_Line_2:UNIT 13, 2 ARTICHOKE HILL</t>
+  </si>
+  <si>
+    <t>Country:United Kingdom</t>
+  </si>
+  <si>
+    <t>IBAN:GB60MHCB40506910804139</t>
+  </si>
+  <si>
+    <t>Agent_Id:MHCBGB2L</t>
+  </si>
+  <si>
+    <t>Instructed_Amount:16</t>
+  </si>
+  <si>
+    <t>Name:MARUBENI EUROPE LIMITED</t>
+  </si>
+  <si>
+    <t>IBAN:GB45MHCB40506910780741</t>
+  </si>
+  <si>
+    <t>Account_Currency:EUR - Euro</t>
+  </si>
+  <si>
+    <t>Beneficiary_BANK_BIC:MHCBGB2L</t>
+  </si>
+  <si>
+    <t>Unstructured_Remittance_Information:UNSTRUCTURED REMITTANCE INFORMATION FIELD</t>
+  </si>
+  <si>
+    <t>Add_And_Verify_Transaction_Summary</t>
+  </si>
+  <si>
+    <t>Credit_Party_Name:MARUBENI EUROPE LIMITED</t>
+  </si>
+  <si>
+    <t>Credit_Party_Account:GB45MHCB40506910780741</t>
+  </si>
+  <si>
+    <t>Credit_Party_Agent_Id:MHCBGB2L</t>
+  </si>
+  <si>
+    <t>Transaction_Amount:16.00</t>
+  </si>
+  <si>
+    <t>Instructed_Currency:EUR</t>
+  </si>
+  <si>
+    <t>End_to_End_Identification:xx999xx</t>
+  </si>
+  <si>
+    <t>Save_Transaction_And_Capture_Instruction</t>
+  </si>
+  <si>
+    <t>Payment Management=&gt;Instructions</t>
+  </si>
+  <si>
+    <t>Verify_Instruction_Details</t>
+  </si>
+  <si>
+    <t>Scheme:Bank</t>
+  </si>
+  <si>
+    <t>Processing_Scheme:SCT</t>
+  </si>
+  <si>
+    <t>Classification:Credit Transfer Initiation</t>
+  </si>
+  <si>
+    <t>Inbound_Outbound:Outbound</t>
+  </si>
+  <si>
+    <t>Direction:Incoming</t>
+  </si>
+  <si>
+    <t>Bank:Mizuho London</t>
+  </si>
+  <si>
+    <t>Status:Awaiting 4-Eye Verification</t>
+  </si>
+  <si>
+    <t>Business_Participant:Manual Entry Participant</t>
+  </si>
+  <si>
+    <t>Settlement_Date:Today</t>
+  </si>
+  <si>
+    <t>Settlement_Amount:16</t>
+  </si>
+  <si>
+    <t>Internal_Reason:OK</t>
+  </si>
+  <si>
+    <t>Approve_Worklist_Item_And_Submit</t>
+  </si>
+  <si>
+    <t>Verification_Message:The Instruction has been approved</t>
+  </si>
+  <si>
+    <t>Verify_Transaction_Table</t>
+  </si>
+  <si>
+    <t>Classification:Credit Transfer</t>
+  </si>
+  <si>
+    <t>Amount:16.00 EUR</t>
+  </si>
+  <si>
+    <t>Status:Created</t>
+  </si>
+  <si>
+    <t>Verify_Instruction_History</t>
+  </si>
+  <si>
+    <t>Status:Accepted</t>
+  </si>
+  <si>
+    <t>Verify_Transaction_Details</t>
+  </si>
+  <si>
+    <t>Settlement_Amount:16.00 EUR</t>
+  </si>
+  <si>
+    <t>Credit_Debit:Credit</t>
+  </si>
+  <si>
+    <t>Status:Processed</t>
+  </si>
+  <si>
+    <t>Debit_Party_Account:GB60MHCB40506910804139</t>
+  </si>
+  <si>
+    <t>Debit_Party_Name:AIP LONDON LIMITED</t>
+  </si>
+  <si>
+    <t>Verify_Transaction_History</t>
+  </si>
+  <si>
+    <t>Event_Desc:AMS Accounting Response|Response OK received for Account Event &lt;x&gt; with details: 00 - Normal</t>
+  </si>
+  <si>
+    <t>Event_Desc:Disposition Check|Valid charges account determined from payment:</t>
+  </si>
+  <si>
+    <t>Event_Desc:4-Eye Verification|4-Eye Verification for the instruction has been approved</t>
+  </si>
+  <si>
+    <t>Event_Desc:Claim Charges|No Charges to Claim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,13 +329,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,18 +361,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -166,10 +391,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -327,7 +552,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -336,13 +561,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -352,7 +577,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -361,7 +586,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -370,7 +595,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -380,12 +605,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -416,7 +641,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -435,7 +660,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -447,133 +672,435 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="49.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="56.85546875" collapsed="true"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="56.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -585,18 +1112,18 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -605,12 +1132,12 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -622,31 +1149,74 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>31001057</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
incremental commit, moved objects into their own classes
</commit_message>
<xml_diff>
--- a/Test_Data/TestData.xlsx
+++ b/Test_Data/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="97">
   <si>
     <t>URL</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>Enter_Credit_Party_Agent_And_Enrich_BIC</t>
+  </si>
+  <si>
+    <t>Search_For_Instruction</t>
   </si>
 </sst>
 </file>
@@ -680,7 +683,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,10 +716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,7 +879,7 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C11" t="s">
@@ -902,7 +905,7 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>61</v>
       </c>
     </row>
@@ -922,34 +925,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" t="s">
-        <v>69</v>
-      </c>
-      <c r="J14" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -957,22 +933,34 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -980,28 +968,22 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
-      </c>
-      <c r="H16" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1009,16 +991,28 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>78</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1026,31 +1020,16 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" t="s">
-        <v>87</v>
-      </c>
-      <c r="H18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I18" t="s">
-        <v>88</v>
-      </c>
-      <c r="J18" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1058,13 +1037,31 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>84</v>
+      </c>
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1072,6 +1069,20 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>